<commit_message>
Fixed part paramters on a few components and added to in-altium BOM
</commit_message>
<xml_diff>
--- a/PDB/PDB_REVS/PDB_V22/PDB_BOM including JLC.xlsx
+++ b/PDB/PDB_REVS/PDB_V22/PDB_BOM including JLC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xxjac\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xxjac\Documents\GitHub\PDB\PDB\PDB_REVS\PDB_V22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{783A222D-67A5-4D23-86A2-84BA2A8C8B67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DB9ADB-82EF-41AD-9CB9-482CCC305815}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18690" yWindow="2895" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PDB_V2" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="383">
   <si>
     <t>Description</t>
   </si>
@@ -1168,6 +1168,12 @@
   </si>
   <si>
     <t>CDRV1</t>
+  </si>
+  <si>
+    <t>Can be bought on JLCPCB</t>
+  </si>
+  <si>
+    <t>Cannot be bought on JLCPCB</t>
   </si>
 </sst>
 </file>
@@ -1433,7 +1439,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1498,6 +1504,8 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1714,10 +1722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W998"/>
+  <dimension ref="A1:W999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1735,621 +1743,597 @@
     <col min="11" max="25" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J2" s="26" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I2" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="J2" s="27" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0.35</v>
-      </c>
-      <c r="I3" s="22">
-        <v>0.35</v>
+        <v>12</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="I3" s="21">
+        <v>0.1</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="I4" s="22">
+        <v>0.35</v>
+      </c>
+      <c r="J4" s="27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="36" t="s">
+        <v>292</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H5" s="4">
         <v>0.46</v>
       </c>
-      <c r="I4" s="21">
+      <c r="I5" s="21">
         <v>0.46</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J5" s="28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="37" t="s">
+    <row r="6" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="37" t="s">
         <v>293</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C6" s="2">
         <v>2</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E6" s="2">
         <v>865230640001</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="F6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H6" s="2">
         <v>0.17</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I6" s="22">
         <v>0.34</v>
       </c>
-      <c r="J5" s="29" t="s">
+      <c r="J6" s="29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="38" t="s">
+    <row r="7" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="38" t="s">
         <v>294</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0.92</v>
-      </c>
-      <c r="I6" s="22">
-        <v>0.92</v>
-      </c>
-      <c r="J6" s="27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="37" t="s">
-        <v>361</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>362</v>
+        <v>29</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>364</v>
+        <v>30</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="H7" s="2">
-        <v>0.53</v>
+        <v>0.92</v>
       </c>
       <c r="I7" s="22">
-        <v>0.53</v>
-      </c>
-      <c r="J7" s="30" t="s">
-        <v>365</v>
+        <v>0.92</v>
+      </c>
+      <c r="J7" s="27" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="37" t="s">
-        <v>297</v>
+        <v>361</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C8" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>34</v>
+        <v>362</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>35</v>
+        <v>363</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>36</v>
+        <v>364</v>
       </c>
       <c r="H8" s="2">
-        <v>0.11</v>
+        <v>0.53</v>
       </c>
       <c r="I8" s="22">
-        <v>0.33</v>
+        <v>0.53</v>
       </c>
       <c r="J8" s="30" t="s">
-        <v>37</v>
+        <v>365</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
+        <v>297</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="I9" s="22">
+        <v>0.33</v>
+      </c>
+      <c r="J9" s="30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C10" s="2">
         <v>1</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="2" t="s">
+      <c r="F10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H10" s="2">
         <v>0.51</v>
       </c>
-      <c r="I9" s="22">
+      <c r="I10" s="22">
         <v>0.51</v>
       </c>
-      <c r="J9" s="30" t="s">
+      <c r="J10" s="30" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="38" t="s">
+    <row r="11" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="38" t="s">
         <v>301</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>298</v>
-      </c>
-      <c r="C10" s="2">
-        <v>2</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0.52</v>
-      </c>
-      <c r="I10" s="22">
-        <v>1.04</v>
-      </c>
-      <c r="J10" s="30" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="39" t="s">
-        <v>373</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>299</v>
       </c>
       <c r="C11" s="2">
         <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="I11" s="22">
+        <v>1.04</v>
+      </c>
+      <c r="J11" s="30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="39" t="s">
+        <v>373</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="2" t="s">
+      <c r="F12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="I11" s="22">
-        <v>0.2</v>
-      </c>
-      <c r="J11" s="30" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="36" t="s">
-        <v>300</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>375</v>
-      </c>
-      <c r="C12" s="2">
-        <v>3</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="H12" s="2">
         <v>0.1</v>
       </c>
       <c r="I12" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="J12" s="30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="36" t="s">
+        <v>300</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>375</v>
+      </c>
+      <c r="C13" s="2">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I13" s="22">
         <v>0.6</v>
       </c>
-      <c r="J12" s="30" t="s">
+      <c r="J13" s="30" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="38" t="s">
+    <row r="14" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="38" t="s">
         <v>366</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C14" s="2">
         <v>1</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="2" t="s">
+      <c r="F14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H14" s="2">
         <v>0.64</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I14" s="22">
         <v>0.64</v>
       </c>
-      <c r="J13" s="30" t="s">
+      <c r="J14" s="30" t="s">
         <v>370</v>
       </c>
-      <c r="K13" s="7"/>
-    </row>
-    <row r="14" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="36" t="s">
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="36" t="s">
         <v>303</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B15" s="20" t="s">
         <v>302</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C15" s="2">
         <v>3</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="2" t="s">
+      <c r="F15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H15" s="2">
         <v>2.5099999999999998</v>
       </c>
-      <c r="I14" s="22">
+      <c r="I15" s="22">
         <v>10.039999999999999</v>
       </c>
-      <c r="J14" s="30" t="s">
+      <c r="J15" s="30" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="37" t="s">
+    <row r="16" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="37" t="s">
         <v>304</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B16" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C16" s="2">
         <v>1</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="2" t="s">
+      <c r="F16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H16" s="2">
         <v>0.89</v>
       </c>
-      <c r="I15" s="22">
+      <c r="I16" s="22">
         <v>0.89</v>
       </c>
-      <c r="J15" s="30" t="s">
+      <c r="J16" s="30" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="36" t="s">
+    <row r="17" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="36" t="s">
         <v>305</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B17" s="20" t="s">
         <v>306</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C17" s="2">
         <v>4</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="2" t="s">
+      <c r="F17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H17" s="2">
         <v>0.46</v>
       </c>
-      <c r="I16" s="22">
+      <c r="I17" s="22">
         <v>1.84</v>
       </c>
-      <c r="J16" s="27" t="s">
+      <c r="J17" s="27" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="37" t="s">
+    <row r="18" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="37" t="s">
         <v>307</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C18" s="2">
         <v>1</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E18" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="2" t="s">
+      <c r="F18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H18" s="2">
         <v>0.48</v>
       </c>
-      <c r="I17" s="22">
+      <c r="I18" s="22">
         <v>0.48</v>
       </c>
-      <c r="J17" s="30" t="s">
+      <c r="J18" s="30" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="39" t="s">
-        <v>308</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>315</v>
-      </c>
-      <c r="C18" s="2">
-        <v>14</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0.65</v>
-      </c>
-      <c r="I18" s="22">
-        <v>9.1</v>
-      </c>
-      <c r="J18" s="30" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="39" t="s">
+        <v>308</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="C19" s="2">
+        <v>14</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="I19" s="22">
+        <v>9.1</v>
+      </c>
+      <c r="J19" s="30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="39" t="s">
         <v>311</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B20" s="20" t="s">
         <v>313</v>
-      </c>
-      <c r="C19" s="2">
-        <v>1</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H19" s="2">
-        <v>0.33</v>
-      </c>
-      <c r="I19" s="22">
-        <v>0.33</v>
-      </c>
-      <c r="J19" s="31" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="37" t="s">
-        <v>312</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="C20" s="2">
         <v>1</v>
@@ -2358,350 +2342,350 @@
         <v>77</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="I20" s="22">
+        <v>0.33</v>
+      </c>
+      <c r="J20" s="31" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="2" t="s">
+      <c r="F21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H21" s="2">
         <v>3.82</v>
       </c>
-      <c r="I20" s="22">
+      <c r="I21" s="22">
         <v>3.82</v>
       </c>
-      <c r="J20" s="30" t="s">
+      <c r="J21" s="30" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="36" t="s">
+    <row r="22" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="B22" s="40" t="s">
         <v>309</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C22" s="2">
         <v>10</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="2" t="s">
+      <c r="F22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H22" s="2">
         <v>0.39</v>
       </c>
-      <c r="I21" s="22">
+      <c r="I22" s="22">
         <v>3.9</v>
       </c>
-      <c r="J21" s="27" t="s">
+      <c r="J22" s="27" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="37" t="s">
-        <v>316</v>
-      </c>
-      <c r="B22" s="40" t="s">
-        <v>376</v>
-      </c>
-      <c r="C22" s="2">
-        <v>2</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H22" s="2">
-        <v>2.83</v>
-      </c>
-      <c r="I22" s="22">
-        <v>5.66</v>
-      </c>
-      <c r="J22" s="30" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="37" t="s">
-        <v>318</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>317</v>
+        <v>316</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>376</v>
       </c>
       <c r="C23" s="2">
         <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H23" s="2">
+        <v>2.83</v>
+      </c>
+      <c r="I23" s="22">
+        <v>5.66</v>
+      </c>
+      <c r="J23" s="30" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="37" t="s">
+        <v>318</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G23" s="8" t="s">
+      <c r="F24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H24" s="2">
         <v>1.5</v>
       </c>
-      <c r="I23" s="22">
+      <c r="I24" s="22">
         <v>5</v>
       </c>
-      <c r="J23" s="30" t="s">
+      <c r="J24" s="30" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="36" t="s">
-        <v>322</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>374</v>
-      </c>
-      <c r="C24" s="2">
-        <v>7</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H24" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="I24" s="22">
-        <v>1.9</v>
-      </c>
-      <c r="J24" s="30" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="36" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>319</v>
+        <v>374</v>
       </c>
       <c r="C25" s="2">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H25" s="2">
         <v>0.1</v>
       </c>
       <c r="I25" s="22">
-        <v>1.3</v>
+        <v>1.9</v>
       </c>
       <c r="J25" s="30" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="36" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>378</v>
+        <v>319</v>
       </c>
       <c r="C26" s="2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H26" s="2">
         <v>0.1</v>
       </c>
       <c r="I26" s="22">
-        <v>0.2</v>
+        <v>1.3</v>
       </c>
       <c r="J26" s="30" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="36" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>320</v>
+        <v>378</v>
       </c>
       <c r="C27" s="2">
         <v>1</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>105</v>
+        <v>51</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H27" s="2">
-        <v>0.41</v>
+        <v>0.1</v>
       </c>
       <c r="I27" s="22">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="J27" s="30" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="36" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C28" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>47</v>
+        <v>105</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H28" s="2">
-        <v>0.34</v>
+        <v>0.41</v>
       </c>
       <c r="I28" s="22">
-        <v>1.7</v>
+        <v>0.82</v>
       </c>
       <c r="J28" s="30" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="36" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="C29" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H29" s="2">
-        <v>0.1</v>
+        <v>0.34</v>
       </c>
       <c r="I29" s="22">
-        <v>0.5</v>
+        <v>1.7</v>
       </c>
       <c r="J29" s="30" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="36" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C30" s="2">
         <v>1</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>116</v>
+        <v>51</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H30" s="2">
         <v>0.1</v>
       </c>
       <c r="I30" s="22">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="J30" s="30" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="36" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C31" s="2">
         <v>1</v>
@@ -2710,13 +2694,13 @@
         <v>116</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H31" s="2">
         <v>0.1</v>
@@ -2725,468 +2709,455 @@
         <v>0.1</v>
       </c>
       <c r="J31" s="30" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="36" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C32" s="2">
         <v>1</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>47</v>
+        <v>116</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H32" s="2">
-        <v>0.36</v>
+        <v>0.1</v>
       </c>
       <c r="I32" s="22">
-        <v>0.36</v>
+        <v>0.1</v>
       </c>
       <c r="J32" s="30" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="36" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>379</v>
+        <v>333</v>
       </c>
       <c r="C33" s="2">
         <v>1</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0.36</v>
+      </c>
+      <c r="I33" s="22">
+        <v>0.36</v>
+      </c>
+      <c r="J33" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="36" t="s">
+        <v>335</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>379</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="F33" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="2" t="s">
+      <c r="F34" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H34" s="2">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I33" s="22">
+      <c r="I34" s="22">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J33" s="30" t="s">
+      <c r="J34" s="30" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="37" t="s">
+    <row r="35" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="37" t="s">
         <v>338</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B35" s="20" t="s">
         <v>377</v>
-      </c>
-      <c r="C34" s="2">
-        <v>3</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="H34" s="2">
-        <v>0.71</v>
-      </c>
-      <c r="I34" s="22">
-        <v>1.76</v>
-      </c>
-      <c r="J34" s="31" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="36" t="s">
-        <v>339</v>
-      </c>
-      <c r="B35" s="20" t="s">
-        <v>337</v>
       </c>
       <c r="C35" s="2">
         <v>3</v>
       </c>
       <c r="D35" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0.71</v>
+      </c>
+      <c r="I35" s="22">
+        <v>1.76</v>
+      </c>
+      <c r="J35" s="31" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="36" t="s">
+        <v>339</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>337</v>
+      </c>
+      <c r="C36" s="2">
+        <v>3</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E36" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="F35" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G35" s="2" t="s">
+      <c r="F36" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="H35" s="2">
+      <c r="H36" s="2">
         <v>0.34</v>
       </c>
-      <c r="I35" s="22">
+      <c r="I36" s="22">
         <v>1.02</v>
       </c>
-      <c r="J35" s="30" t="s">
+      <c r="J36" s="30" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="36" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="39" t="s">
+    <row r="37" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="39" t="s">
         <v>341</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B37" s="20" t="s">
         <v>340</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C37" s="2">
         <v>2</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="E37" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="F36" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G36" s="2" t="s">
+      <c r="F37" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="H36" s="2">
+      <c r="H37" s="2">
         <v>0.1</v>
       </c>
-      <c r="I36" s="22">
+      <c r="I37" s="22">
         <v>0.3</v>
       </c>
-      <c r="J36" s="30" t="s">
+      <c r="J37" s="30" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="37" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="36" t="s">
+    <row r="38" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="36" t="s">
         <v>343</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B38" s="20" t="s">
         <v>342</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C38" s="2">
         <v>8</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="E38" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="F37" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G37" s="2" t="s">
+      <c r="F38" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H38" s="2">
         <v>0.34</v>
       </c>
-      <c r="I37" s="22">
+      <c r="I38" s="22">
         <v>1.02</v>
       </c>
-      <c r="J37" s="30" t="s">
+      <c r="J38" s="30" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="36" t="s">
+    <row r="39" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="36" t="s">
         <v>344</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B39" s="20" t="s">
         <v>345</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C39" s="2">
         <v>2</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="E39" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="F38" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G38" s="2" t="s">
+      <c r="F39" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="H38" s="2">
+      <c r="H39" s="2">
         <v>0.11</v>
       </c>
-      <c r="I38" s="22">
+      <c r="I39" s="22">
         <v>0.22</v>
       </c>
-      <c r="J38" s="30" t="s">
+      <c r="J39" s="30" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="39" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="37" t="s">
+    <row r="40" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="37" t="s">
         <v>346</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="B40" s="20" t="s">
         <v>350</v>
       </c>
-      <c r="C39" s="20" t="s">
+      <c r="C40" s="20" t="s">
         <v>351</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="E40" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F39" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G39" s="2" t="s">
+      <c r="F40" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="H39" s="2">
+      <c r="H40" s="2">
         <v>6.36</v>
       </c>
-      <c r="I39" s="22">
+      <c r="I40" s="22">
         <v>19.079999999999998</v>
       </c>
-      <c r="J39" s="27" t="s">
+      <c r="J40" s="27" t="s">
         <v>347</v>
-      </c>
-    </row>
-    <row r="40" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="37" t="s">
-        <v>353</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="C40" s="2">
-        <v>1</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="H40" s="2">
-        <v>1.08</v>
-      </c>
-      <c r="I40" s="22">
-        <v>1.08</v>
-      </c>
-      <c r="J40" s="30" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="41" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="37" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>352</v>
+        <v>144</v>
       </c>
       <c r="C41" s="2">
         <v>1</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>62</v>
+        <v>145</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H41" s="2">
-        <v>0.73</v>
+        <v>1.08</v>
       </c>
       <c r="I41" s="22">
-        <v>1.46</v>
+        <v>1.08</v>
       </c>
       <c r="J41" s="30" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="42" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="37" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>152</v>
+        <v>352</v>
       </c>
       <c r="C42" s="2">
         <v>1</v>
       </c>
       <c r="D42" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="H42" s="2">
+        <v>0.73</v>
+      </c>
+      <c r="I42" s="22">
+        <v>1.46</v>
+      </c>
+      <c r="J42" s="30" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="37" t="s">
+        <v>355</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="C43" s="2">
+        <v>1</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E42" s="41" t="s">
+      <c r="E43" s="41" t="s">
         <v>154</v>
       </c>
-      <c r="F42" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G42" s="2" t="s">
+      <c r="F43" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H43" s="2">
         <v>12.5</v>
       </c>
-      <c r="I42" s="22">
+      <c r="I43" s="22">
         <v>12.5</v>
       </c>
-      <c r="J42" s="32" t="s">
+      <c r="J43" s="32" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="43" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="42" t="s">
+    <row r="44" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="42" t="s">
         <v>358</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="B44" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="C43" s="11">
+      <c r="C44" s="11">
         <v>3</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D44" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="E44" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="F43" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G43" s="11" t="s">
+      <c r="F44" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="H43" s="11">
+      <c r="H44" s="11">
         <v>0.43</v>
       </c>
-      <c r="I43" s="23">
+      <c r="I44" s="23">
         <v>1.29</v>
       </c>
-      <c r="J43" s="27" t="s">
+      <c r="J44" s="27" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="43" t="s">
+    <row r="45" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="43" t="s">
         <v>160</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="B45" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="C44" s="13">
+      <c r="C45" s="13">
         <v>1</v>
       </c>
-      <c r="D44" s="13" t="s">
+      <c r="D45" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="E44" s="14" t="s">
+      <c r="E45" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="F44" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G44" s="14" t="s">
+      <c r="F45" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="H44" s="13">
+      <c r="H45" s="13">
         <v>0.42</v>
       </c>
-      <c r="I44" s="24">
+      <c r="I45" s="24">
         <v>0.42</v>
       </c>
-      <c r="J44" s="33" t="s">
+      <c r="J45" s="33" t="s">
         <v>165</v>
-      </c>
-      <c r="K44" s="10"/>
-      <c r="L44" s="10"/>
-      <c r="M44" s="10"/>
-      <c r="N44" s="10"/>
-      <c r="O44" s="10"/>
-      <c r="P44" s="10"/>
-      <c r="Q44" s="10"/>
-      <c r="R44" s="10"/>
-      <c r="S44" s="10"/>
-      <c r="T44" s="10"/>
-      <c r="U44" s="10"/>
-      <c r="V44" s="10"/>
-      <c r="W44" s="10"/>
-    </row>
-    <row r="45" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="45" t="s">
-        <v>166</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="C45" s="13">
-        <v>2</v>
-      </c>
-      <c r="D45" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="F45" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G45" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="H45" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="I45" s="24">
-        <v>0.2</v>
-      </c>
-      <c r="J45" s="34" t="s">
-        <v>170</v>
       </c>
       <c r="K45" s="10"/>
       <c r="L45" s="10"/>
@@ -3204,34 +3175,34 @@
     </row>
     <row r="46" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="45" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C46" s="13">
-        <v>1</v>
-      </c>
-      <c r="D46" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E46" s="13" t="s">
-        <v>173</v>
+      <c r="E46" s="14" t="s">
+        <v>168</v>
       </c>
       <c r="F46" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G46" s="16" t="s">
-        <v>174</v>
+      <c r="G46" s="13" t="s">
+        <v>169</v>
       </c>
       <c r="H46" s="13">
-        <v>0.28000000000000003</v>
+        <v>0.1</v>
       </c>
       <c r="I46" s="24">
-        <v>0.28000000000000003</v>
+        <v>0.2</v>
       </c>
       <c r="J46" s="34" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="K46" s="10"/>
       <c r="L46" s="10"/>
@@ -3249,10 +3220,10 @@
     </row>
     <row r="47" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="45" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C47" s="13">
         <v>1</v>
@@ -3261,22 +3232,22 @@
         <v>9</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F47" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G47" s="13" t="s">
-        <v>179</v>
+      <c r="G47" s="16" t="s">
+        <v>174</v>
       </c>
       <c r="H47" s="13">
-        <v>0.1</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="I47" s="24">
-        <v>0.1</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="J47" s="34" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="K47" s="10"/>
       <c r="L47" s="10"/>
@@ -3293,35 +3264,35 @@
       <c r="W47" s="10"/>
     </row>
     <row r="48" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="44" t="s">
-        <v>181</v>
+      <c r="A48" s="45" t="s">
+        <v>176</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C48" s="13">
         <v>1</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>145</v>
+        <v>9</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F48" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G48" s="14" t="s">
-        <v>184</v>
+      <c r="G48" s="13" t="s">
+        <v>179</v>
       </c>
       <c r="H48" s="13">
-        <v>0.86</v>
+        <v>0.1</v>
       </c>
       <c r="I48" s="24">
-        <v>0.86</v>
-      </c>
-      <c r="J48" s="33" t="s">
-        <v>185</v>
+        <v>0.1</v>
+      </c>
+      <c r="J48" s="34" t="s">
+        <v>180</v>
       </c>
       <c r="K48" s="10"/>
       <c r="L48" s="10"/>
@@ -3339,34 +3310,34 @@
     </row>
     <row r="49" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="44" t="s">
-        <v>359</v>
+        <v>181</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C49" s="13">
         <v>1</v>
       </c>
-      <c r="D49" s="15" t="s">
-        <v>47</v>
+      <c r="D49" s="13" t="s">
+        <v>145</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F49" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G49" s="15" t="s">
-        <v>188</v>
+      <c r="G49" s="14" t="s">
+        <v>184</v>
       </c>
       <c r="H49" s="13">
-        <v>0.39</v>
+        <v>0.86</v>
       </c>
       <c r="I49" s="24">
-        <v>0.39</v>
+        <v>0.86</v>
       </c>
       <c r="J49" s="33" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="K49" s="10"/>
       <c r="L49" s="10"/>
@@ -3383,35 +3354,35 @@
       <c r="W49" s="10"/>
     </row>
     <row r="50" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="45" t="s">
-        <v>190</v>
+      <c r="A50" s="44" t="s">
+        <v>359</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C50" s="13">
         <v>1</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="14" t="s">
-        <v>192</v>
+        <v>47</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>187</v>
       </c>
       <c r="F50" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G50" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="H50" s="35">
-        <v>1.32</v>
+      <c r="G50" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="H50" s="13">
+        <v>0.39</v>
       </c>
       <c r="I50" s="24">
-        <v>1.32</v>
+        <v>0.39</v>
       </c>
       <c r="J50" s="33" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="K50" s="10"/>
       <c r="L50" s="10"/>
@@ -3429,34 +3400,34 @@
     </row>
     <row r="51" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="45" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C51" s="13">
         <v>1</v>
       </c>
-      <c r="D51" s="17" t="s">
-        <v>197</v>
+      <c r="D51" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="F51" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G51" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="H51" s="15">
-        <v>0.27</v>
+      <c r="G51" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="H51" s="35">
+        <v>1.32</v>
       </c>
       <c r="I51" s="24">
-        <v>0.27</v>
+        <v>1.32</v>
       </c>
       <c r="J51" s="33" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="K51" s="10"/>
       <c r="L51" s="10"/>
@@ -3474,34 +3445,34 @@
     </row>
     <row r="52" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="45" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C52" s="13">
         <v>1</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="E52" s="14" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="F52" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G52" s="14" t="s">
-        <v>205</v>
-      </c>
-      <c r="H52" s="13">
-        <v>0.26</v>
+        <v>199</v>
+      </c>
+      <c r="H52" s="15">
+        <v>0.27</v>
       </c>
       <c r="I52" s="24">
-        <v>0.26</v>
+        <v>0.27</v>
       </c>
       <c r="J52" s="33" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="K52" s="10"/>
       <c r="L52" s="10"/>
@@ -3519,10 +3490,10 @@
     </row>
     <row r="53" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="45" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C53" s="13">
         <v>1</v>
@@ -3531,22 +3502,22 @@
         <v>203</v>
       </c>
       <c r="E53" s="14" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F53" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G53" s="14" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H53" s="13">
-        <v>0.12</v>
+        <v>0.26</v>
       </c>
       <c r="I53" s="24">
-        <v>0.12</v>
+        <v>0.26</v>
       </c>
       <c r="J53" s="33" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="K53" s="10"/>
       <c r="L53" s="10"/>
@@ -3563,35 +3534,35 @@
       <c r="W53" s="10"/>
     </row>
     <row r="54" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="46" t="s">
-        <v>212</v>
+      <c r="A54" s="45" t="s">
+        <v>207</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C54" s="13">
-        <v>2</v>
-      </c>
-      <c r="D54" s="18" t="s">
-        <v>73</v>
+        <v>1</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>203</v>
       </c>
       <c r="E54" s="14" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="F54" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G54" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="H54" s="15">
-        <v>0.35</v>
+        <v>210</v>
+      </c>
+      <c r="H54" s="13">
+        <v>0.12</v>
       </c>
       <c r="I54" s="24">
-        <v>0.7</v>
+        <v>0.12</v>
       </c>
       <c r="J54" s="33" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="K54" s="10"/>
       <c r="L54" s="10"/>
@@ -3608,35 +3579,35 @@
       <c r="W54" s="10"/>
     </row>
     <row r="55" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="38" t="s">
-        <v>371</v>
+      <c r="A55" s="46" t="s">
+        <v>212</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>372</v>
+        <v>213</v>
       </c>
       <c r="C55" s="13">
-        <v>1</v>
-      </c>
-      <c r="D55" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="E55" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="F55" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="G55" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="H55" s="13">
-        <v>6.13</v>
+        <v>2</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="F55" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G55" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="H55" s="15">
+        <v>0.35</v>
       </c>
       <c r="I55" s="24">
-        <v>6.13</v>
+        <v>0.7</v>
       </c>
       <c r="J55" s="33" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="K55" s="10"/>
       <c r="L55" s="10"/>
@@ -3653,35 +3624,35 @@
       <c r="W55" s="10"/>
     </row>
     <row r="56" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="47" t="s">
-        <v>221</v>
+      <c r="A56" s="38" t="s">
+        <v>371</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>222</v>
+        <v>372</v>
       </c>
       <c r="C56" s="13">
-        <v>3</v>
-      </c>
-      <c r="D56" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="E56" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="F56" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G56" s="14" t="s">
-        <v>225</v>
+        <v>1</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="E56" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="F56" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="G56" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="H56" s="13">
-        <v>0.65</v>
+        <v>6.13</v>
       </c>
       <c r="I56" s="24">
-        <v>1.95</v>
+        <v>6.13</v>
       </c>
       <c r="J56" s="33" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="K56" s="10"/>
       <c r="L56" s="10"/>
@@ -3698,35 +3669,35 @@
       <c r="W56" s="10"/>
     </row>
     <row r="57" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="44" t="s">
-        <v>227</v>
+      <c r="A57" s="47" t="s">
+        <v>221</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C57" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D57" s="18" t="s">
         <v>223</v>
       </c>
       <c r="E57" s="14" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G57" s="14" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="H57" s="13">
-        <v>1.76</v>
+        <v>0.65</v>
       </c>
       <c r="I57" s="24">
-        <v>3.52</v>
+        <v>1.95</v>
       </c>
       <c r="J57" s="33" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="K57" s="10"/>
       <c r="L57" s="10"/>
@@ -3744,34 +3715,34 @@
     </row>
     <row r="58" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="44" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C58" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D58" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="E58" s="13" t="s">
-        <v>234</v>
+      <c r="E58" s="14" t="s">
+        <v>229</v>
       </c>
       <c r="F58" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G58" s="14" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="H58" s="13">
-        <v>1.54</v>
+        <v>1.76</v>
       </c>
       <c r="I58" s="24">
-        <v>1.54</v>
+        <v>3.52</v>
       </c>
       <c r="J58" s="33" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="K58" s="10"/>
       <c r="L58" s="10"/>
@@ -3789,34 +3760,34 @@
     </row>
     <row r="59" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="44" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C59" s="13">
         <v>1</v>
       </c>
-      <c r="D59" s="15" t="s">
-        <v>239</v>
+      <c r="D59" s="18" t="s">
+        <v>223</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G59" s="13" t="s">
-        <v>241</v>
+      <c r="G59" s="14" t="s">
+        <v>235</v>
       </c>
       <c r="H59" s="13">
-        <v>15.99</v>
+        <v>1.54</v>
       </c>
       <c r="I59" s="24">
-        <v>15.99</v>
+        <v>1.54</v>
       </c>
       <c r="J59" s="33" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="K59" s="10"/>
       <c r="L59" s="10"/>
@@ -3833,35 +3804,35 @@
       <c r="W59" s="10"/>
     </row>
     <row r="60" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="45" t="s">
-        <v>360</v>
+      <c r="A60" s="44" t="s">
+        <v>237</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C60" s="13">
         <v>1</v>
       </c>
-      <c r="D60" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E60" s="14" t="s">
-        <v>244</v>
+      <c r="D60" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="E60" s="13" t="s">
+        <v>240</v>
       </c>
       <c r="F60" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G60" s="14" t="s">
-        <v>245</v>
+      <c r="G60" s="13" t="s">
+        <v>241</v>
       </c>
       <c r="H60" s="13">
-        <v>0.1</v>
+        <v>15.99</v>
       </c>
       <c r="I60" s="24">
-        <v>0.1</v>
+        <v>15.99</v>
       </c>
       <c r="J60" s="33" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="K60" s="10"/>
       <c r="L60" s="10"/>
@@ -3879,34 +3850,34 @@
     </row>
     <row r="61" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="45" t="s">
-        <v>247</v>
+        <v>360</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="C61" s="13">
         <v>1</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>116</v>
+        <v>51</v>
       </c>
       <c r="E61" s="14" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="F61" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G61" s="14" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="H61" s="13">
-        <v>0.56000000000000005</v>
+        <v>0.1</v>
       </c>
       <c r="I61" s="24">
-        <v>0.56000000000000005</v>
+        <v>0.1</v>
       </c>
       <c r="J61" s="33" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="K61" s="10"/>
       <c r="L61" s="10"/>
@@ -3924,34 +3895,34 @@
     </row>
     <row r="62" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="45" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C62" s="13">
-        <v>2</v>
-      </c>
-      <c r="D62" s="15" t="s">
-        <v>51</v>
+        <v>1</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>116</v>
       </c>
       <c r="E62" s="14" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="F62" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G62" s="14" t="s">
-        <v>255</v>
-      </c>
-      <c r="H62" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="I62" s="25">
-        <v>0.2</v>
+        <v>250</v>
+      </c>
+      <c r="H62" s="13">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I62" s="24">
+        <v>0.56000000000000005</v>
       </c>
       <c r="J62" s="33" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="K62" s="10"/>
       <c r="L62" s="10"/>
@@ -3969,34 +3940,34 @@
     </row>
     <row r="63" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="45" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C63" s="13">
-        <v>1</v>
-      </c>
-      <c r="D63" s="18" t="s">
-        <v>47</v>
+        <v>2</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="E63" s="14" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G63" s="14" t="s">
-        <v>260</v>
-      </c>
-      <c r="H63" s="13">
-        <v>0.41</v>
-      </c>
-      <c r="I63" s="24">
-        <v>0.41</v>
+        <v>255</v>
+      </c>
+      <c r="H63" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="I63" s="25">
+        <v>0.2</v>
       </c>
       <c r="J63" s="33" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="K63" s="10"/>
       <c r="L63" s="10"/>
@@ -4014,34 +3985,34 @@
     </row>
     <row r="64" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="45" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="C64" s="13">
         <v>1</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E64" s="14" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="F64" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G64" s="14" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="H64" s="13">
-        <v>0.1</v>
+        <v>0.41</v>
       </c>
       <c r="I64" s="24">
-        <v>0.1</v>
+        <v>0.41</v>
       </c>
       <c r="J64" s="33" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="K64" s="10"/>
       <c r="L64" s="10"/>
@@ -4059,10 +4030,10 @@
     </row>
     <row r="65" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="45" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C65" s="13">
         <v>1</v>
@@ -4071,13 +4042,13 @@
         <v>51</v>
       </c>
       <c r="E65" s="14" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G65" s="14" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="H65" s="13">
         <v>0.1</v>
@@ -4086,7 +4057,7 @@
         <v>0.1</v>
       </c>
       <c r="J65" s="33" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="K65" s="10"/>
       <c r="L65" s="10"/>
@@ -4104,25 +4075,25 @@
     </row>
     <row r="66" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="45" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C66" s="13">
         <v>1</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>274</v>
+        <v>51</v>
       </c>
       <c r="E66" s="14" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="F66" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G66" s="14" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="H66" s="13">
         <v>0.1</v>
@@ -4131,7 +4102,7 @@
         <v>0.1</v>
       </c>
       <c r="J66" s="33" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="K66" s="10"/>
       <c r="L66" s="10"/>
@@ -4149,34 +4120,34 @@
     </row>
     <row r="67" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="45" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>112</v>
+        <v>273</v>
       </c>
       <c r="C67" s="13">
         <v>1</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>116</v>
+        <v>274</v>
       </c>
       <c r="E67" s="14" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F67" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G67" s="14" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="H67" s="13">
-        <v>0.56000000000000005</v>
+        <v>0.1</v>
       </c>
       <c r="I67" s="24">
-        <v>0.56000000000000005</v>
+        <v>0.1</v>
       </c>
       <c r="J67" s="33" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="K67" s="10"/>
       <c r="L67" s="10"/>
@@ -4193,35 +4164,35 @@
       <c r="W67" s="10"/>
     </row>
     <row r="68" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="44" t="s">
-        <v>282</v>
-      </c>
-      <c r="B68" s="15" t="s">
-        <v>283</v>
+      <c r="A68" s="45" t="s">
+        <v>278</v>
+      </c>
+      <c r="B68" s="13" t="s">
+        <v>112</v>
       </c>
       <c r="C68" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>284</v>
+        <v>116</v>
       </c>
       <c r="E68" s="14" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="F68" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G68" s="14" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="H68" s="13">
-        <v>0.59</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="I68" s="24">
-        <v>1.18</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="J68" s="33" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="K68" s="10"/>
       <c r="L68" s="10"/>
@@ -4238,17 +4209,61 @@
       <c r="W68" s="10"/>
     </row>
     <row r="69" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="48" t="s">
+      <c r="A69" s="44" t="s">
+        <v>282</v>
+      </c>
+      <c r="B69" s="15" t="s">
+        <v>283</v>
+      </c>
+      <c r="C69" s="13">
+        <v>2</v>
+      </c>
+      <c r="D69" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="E69" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="F69" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G69" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="H69" s="13">
+        <v>0.59</v>
+      </c>
+      <c r="I69" s="24">
+        <v>1.18</v>
+      </c>
+      <c r="J69" s="33" t="s">
+        <v>287</v>
+      </c>
+      <c r="K69" s="10"/>
+      <c r="L69" s="10"/>
+      <c r="M69" s="10"/>
+      <c r="N69" s="10"/>
+      <c r="O69" s="10"/>
+      <c r="P69" s="10"/>
+      <c r="Q69" s="10"/>
+      <c r="R69" s="10"/>
+      <c r="S69" s="10"/>
+      <c r="T69" s="10"/>
+      <c r="U69" s="10"/>
+      <c r="V69" s="10"/>
+      <c r="W69" s="10"/>
+    </row>
+    <row r="70" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B70" s="48" t="s">
         <v>380</v>
       </c>
-      <c r="C69" s="48">
+      <c r="C70" s="48">
         <v>1</v>
       </c>
-      <c r="D69" s="10"/>
-      <c r="E69" s="49"/>
-      <c r="F69" s="48"/>
-    </row>
-    <row r="70" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="49"/>
+      <c r="F70" s="48"/>
+    </row>
     <row r="71" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="72" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="73" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5177,83 +5192,84 @@
     <row r="996" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="997" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="999" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="J3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="J4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="J5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="J6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="J8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="J9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="J10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="J11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="J12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="J14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="J15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="J16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="J17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="J18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="J20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="J22" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="J23" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="J24" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="J25" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="J26" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="J27" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="J28" r:id="rId23" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="J29" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="J30" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="J31" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="J32" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="J33" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="J35" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="J36" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="J37" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="J38" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="J40" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="J41" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="J43" r:id="rId35" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="J44" r:id="rId36" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="J45" r:id="rId37" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="J46" r:id="rId38" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="J47" r:id="rId39" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="J48" r:id="rId40" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="J49" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="J50" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="J51" r:id="rId43" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="J52" r:id="rId44" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="J53" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="D54" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="J54" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="J55" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="D56" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="J56" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="D57" r:id="rId51" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="J57" r:id="rId52" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="D58" r:id="rId53" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="J58" r:id="rId54" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="J59" r:id="rId55" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="D60" r:id="rId56" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="J60" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="D61" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="J61" r:id="rId59" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="J62" r:id="rId60" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="D63" r:id="rId61" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="J63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="D64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="J64" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="D65" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="J65" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="D66" r:id="rId67" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="J66" r:id="rId68" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="D67" r:id="rId69" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="J67" r:id="rId70" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="D68" r:id="rId71" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="J68" r:id="rId72" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="J19" r:id="rId73" xr:uid="{290EA8EE-7DA5-4CF6-BE12-4BB0E272E016}"/>
-    <hyperlink ref="J21" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="J34" r:id="rId75" xr:uid="{F85FE9F8-E425-48FF-89D4-A25158ED205B}"/>
+    <hyperlink ref="J3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="J4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="J6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="J7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="J9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="J10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="J11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="J12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="J13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="J15" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="J16" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="J17" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="J18" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="J19" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="J21" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="J23" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="J24" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="J25" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="J26" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="J27" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="J28" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="J29" r:id="rId22" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="J30" r:id="rId23" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="J31" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="J32" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="J33" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="J34" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="J36" r:id="rId28" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="J37" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="J38" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="J39" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="J41" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="J42" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="J44" r:id="rId34" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="J45" r:id="rId35" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="J46" r:id="rId36" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="J47" r:id="rId37" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="J48" r:id="rId38" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="J49" r:id="rId39" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="J50" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="J51" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="J52" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="J53" r:id="rId43" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="J54" r:id="rId44" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="D55" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="J55" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="J56" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="D57" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="J57" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="D58" r:id="rId50" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="J58" r:id="rId51" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="D59" r:id="rId52" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="J59" r:id="rId53" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="J60" r:id="rId54" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="D61" r:id="rId55" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="J61" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="D62" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="J62" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="J63" r:id="rId59" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="D64" r:id="rId60" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="J64" r:id="rId61" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="D65" r:id="rId62" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="J65" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="D66" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="J66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="D67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="J67" r:id="rId67" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="D68" r:id="rId68" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="J68" r:id="rId69" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="D69" r:id="rId70" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="J69" r:id="rId71" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="J20" r:id="rId72" xr:uid="{290EA8EE-7DA5-4CF6-BE12-4BB0E272E016}"/>
+    <hyperlink ref="J22" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="J35" r:id="rId74" xr:uid="{F85FE9F8-E425-48FF-89D4-A25158ED205B}"/>
+    <hyperlink ref="J5" r:id="rId75" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId76"/>

</xml_diff>